<commit_message>
Create collection 18MoreAnd21andLess on MongoDB
</commit_message>
<xml_diff>
--- a/df_1.xlsx
+++ b/df_1.xlsx
@@ -80,7 +80,7 @@
   <cols>
     <col min="5" max="5" hidden="0" bestFit="1" customWidth="1" width="20.714286" style="2"/>
     <col min="6" max="6" hidden="0" bestFit="1" customWidth="1" width="19.714286" style="2"/>
-    <col min="7" max="7" hidden="0" bestFit="1" customWidth="1" width="11.714286" style="2"/>
+    <col min="7" max="7" hidden="0" bestFit="1" customWidth="1" width="19.714286" style="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -146,7 +146,7 @@
         <v>44562.40638888889</v>
       </c>
       <c r="G2" s="4">
-        <v>0.375</v>
+        <v>44562.375</v>
       </c>
     </row>
     <row r="3">
@@ -175,7 +175,7 @@
         <v>44562.49334490741</v>
       </c>
       <c r="G3" s="4">
-        <v>0.38541666666666674</v>
+        <v>44562.385416666664</v>
       </c>
     </row>
     <row r="4">
@@ -205,7 +205,7 @@
       </c>
       <c r="G4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve"/>
+          <t xml:space="preserve">-</t>
         </is>
       </c>
     </row>
@@ -236,7 +236,7 @@
       </c>
       <c r="G5" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve"/>
+          <t xml:space="preserve">-</t>
         </is>
       </c>
     </row>
@@ -266,7 +266,7 @@
         <v>44562.49594907407</v>
       </c>
       <c r="G6" s="4">
-        <v>0.375</v>
+        <v>44562.375</v>
       </c>
     </row>
     <row r="7">
@@ -295,7 +295,7 @@
         <v>44562.414351851854</v>
       </c>
       <c r="G7" s="4">
-        <v>0.38541666666666674</v>
+        <v>44562.385416666664</v>
       </c>
     </row>
     <row r="8">
@@ -324,7 +324,7 @@
         <v>44562.411631944444</v>
       </c>
       <c r="G8" s="4">
-        <v>0.38541666666666674</v>
+        <v>44562.385416666664</v>
       </c>
     </row>
   </sheetData>

</xml_diff>